<commit_message>
Works for artists, not for albums
</commit_message>
<xml_diff>
--- a/fetchtimingmeasurements.xlsx
+++ b/fetchtimingmeasurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\GitHub\music_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C9A8C04-795E-40F4-B9A1-AE076C93BD7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13160613-11A9-46AE-9DC4-EB3A755965C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBC5AB41-BB19-4772-8C3A-EFBF04F15655}"/>
+    <workbookView xWindow="5460" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{DBC5AB41-BB19-4772-8C3A-EFBF04F15655}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Start Time</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Full Local Files Implementation 5</t>
+  </si>
+  <si>
+    <t>Local File</t>
+  </si>
+  <si>
+    <t>Artists and Albums from single file (didn't load properly</t>
   </si>
 </sst>
 </file>
@@ -94,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="hh:mm:ss.000"/>
+    <numFmt numFmtId="164" formatCode="hh:mm:ss.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,7 +139,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E4B70F-7D95-4EC5-A7F2-1ACCEF3FE61C}">
-  <dimension ref="A2:D28"/>
+  <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +505,7 @@
         <v>0.74371346064814814</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D7" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D6" si="0">C4-B4</f>
         <v>1.2397106481482068E-3</v>
       </c>
     </row>
@@ -564,7 +570,7 @@
         <v>0.75156790509259253</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D8:D28" si="1">C9-B9</f>
+        <f t="shared" ref="D9:D28" si="1">C9-B9</f>
         <v>1.2255787037035448E-3</v>
       </c>
     </row>
@@ -728,6 +734,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
       <c r="B24" s="1">
         <v>0.87221223379629631</v>
       </c>
@@ -740,28 +749,83 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.55480302083333333</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.55509247685185181</v>
+      </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8945601851848579E-4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>